<commit_message>
added simply decision tree model
</commit_message>
<xml_diff>
--- a/data-dictionary.xlsx
+++ b/data-dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\engaged_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FD9608-B986-4595-9D08-2EABB5D72625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1D7236-C471-4357-A6D4-222D2C727340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
   <si>
     <t>api_variable_name</t>
   </si>
@@ -424,6 +424,21 @@
   </si>
   <si>
     <t>"1": "Less Than $5,000", "2": "5,000 To 7,499", "3": "7,500 To 9,999", "4": "10,000 To 12,499", "5": "12,500 To 14,999", "6": "15,000 To 19,999", "7": "20,000 To 24,999", "8": "25,000 To 29,999", "9": "30,000 To 34,999", "10": "35,000 To 39,999", "11": "40,000 To 49,999", "12": "50,000 To 59,999", "13": "60,000 To 74,999", "14": "75,000 To 99,999", "15": "100,000 To 149,999", "16": "150,000 or More"</t>
+  </si>
+  <si>
+    <t>PESD1</t>
+  </si>
+  <si>
+    <t>how_disability_affects_ability_to_work</t>
+  </si>
+  <si>
+    <t>How Disability Affects Ability to Work</t>
+  </si>
+  <si>
+    <t>Indicates the severity at which an individuals dissability affects their ability to work</t>
+  </si>
+  <si>
+    <t>"1":"No Difficulty","2":"A Little Difficulty","3":"Moderate Difficulty","4":"Severe Difficulty"</t>
   </si>
 </sst>
 </file>
@@ -753,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -809,58 +824,58 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="13.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>91</v>
       </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
       <c r="E4" t="s">
         <v>85</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
         <v>85</v>
@@ -871,16 +886,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
         <v>85</v>
@@ -891,16 +906,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
         <v>85</v>
@@ -911,16 +926,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" t="s">
         <v>85</v>
@@ -931,16 +946,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
         <v>85</v>
@@ -951,36 +966,36 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" t="s">
         <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
         <v>85</v>
@@ -991,16 +1006,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
         <v>85</v>
@@ -1011,16 +1026,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
         <v>85</v>
@@ -1031,16 +1046,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
         <v>85</v>
@@ -1051,76 +1066,76 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" t="s">
         <v>86</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" t="s">
         <v>86</v>
       </c>
       <c r="F17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E18" t="s">
         <v>86</v>
@@ -1131,16 +1146,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s">
         <v>86</v>
@@ -1151,16 +1166,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
         <v>86</v>
@@ -1171,16 +1186,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" t="s">
         <v>86</v>
@@ -1191,16 +1206,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E22" t="s">
         <v>86</v>
@@ -1211,16 +1226,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
         <v>86</v>
@@ -1231,16 +1246,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E24" t="s">
         <v>86</v>
@@ -1251,121 +1266,141 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F25" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F28" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E29" t="s">
         <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>